<commit_message>
Unit teszt 8 gomb
</commit_message>
<xml_diff>
--- a/Dokumentáció/Tesztbeosztás táblázat.xlsx
+++ b/Dokumentáció/Tesztbeosztás táblázat.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EKE\RFT\beadandó\RFT_project\Dokumentáció\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szicsak98\Documents\GitHub\RFT_project\Dokumentáció\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>Teszt szám</t>
   </si>
@@ -87,13 +87,22 @@
   </si>
   <si>
     <t>7 gomb</t>
+  </si>
+  <si>
+    <t>Szicsák Bence</t>
+  </si>
+  <si>
+    <t>Igen</t>
+  </si>
+  <si>
+    <t>8 gomb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +124,13 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -214,34 +230,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -541,41 +543,41 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" style="4"/>
     <col min="7" max="7" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="8" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
@@ -589,7 +591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -610,7 +612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -631,7 +633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -652,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -673,7 +675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -694,7 +696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -715,7 +717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -736,7 +738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -757,20 +759,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44194</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -783,7 +795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -796,7 +808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -809,7 +821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -822,7 +834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -835,7 +847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -848,7 +860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -861,7 +873,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -874,7 +886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -887,7 +899,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -900,7 +912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -913,7 +925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -926,7 +938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -939,7 +951,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -952,7 +964,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -965,7 +977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -978,7 +990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -991,7 +1003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -1004,7 +1016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -1017,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -1043,7 +1055,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -1059,10 +1071,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G3:G32">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Nem sikerült"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Sikerült"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
9 gomb Unit teszt
</commit_message>
<xml_diff>
--- a/Dokumentáció/Tesztbeosztás táblázat.xlsx
+++ b/Dokumentáció/Tesztbeosztás táblázat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>Teszt szám</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>8 gomb</t>
+  </si>
+  <si>
+    <t>9 gomb</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -237,6 +240,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -558,26 +567,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
@@ -786,13 +795,23 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>11</v>
+      <c r="B12" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="22">
+        <v>44195</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
törlés gomb Unit teszt
</commit_message>
<xml_diff>
--- a/Dokumentáció/Tesztbeosztás táblázat.xlsx
+++ b/Dokumentáció/Tesztbeosztás táblázat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
   <si>
     <t>Teszt szám</t>
   </si>
@@ -99,13 +99,16 @@
   </si>
   <si>
     <t>9 gomb</t>
+  </si>
+  <si>
+    <t>Törlés gomb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +134,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="238"/>
@@ -171,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,6 +256,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -552,7 +571,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -567,26 +586,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
@@ -818,13 +837,23 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>11</v>
+      <c r="B13" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="25">
+        <v>44196</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Egész törlés gomb Unit teszt
</commit_message>
<xml_diff>
--- a/Dokumentáció/Tesztbeosztás táblázat.xlsx
+++ b/Dokumentáció/Tesztbeosztás táblázat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
   <si>
     <t>Teszt szám</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Törlés gomb</t>
+  </si>
+  <si>
+    <t>Egész törles</t>
   </si>
 </sst>
 </file>
@@ -246,25 +249,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,7 +574,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -586,26 +589,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
@@ -806,7 +809,7 @@
       <c r="F11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="22" t="s">
         <v>12</v>
       </c>
     </row>
@@ -817,8 +820,8 @@
       <c r="B12" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="22">
-        <v>44195</v>
+      <c r="C12" s="25">
+        <v>44194</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>8</v>
@@ -837,22 +840,22 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="25">
-        <v>44196</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="24" t="s">
+        <v>44194</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="23" t="s">
         <v>12</v>
       </c>
     </row>
@@ -860,13 +863,23 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>11</v>
+      <c r="B14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="25">
+        <v>44194</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>